<commit_message>
List works (with some known issues)
</commit_message>
<xml_diff>
--- a/testdata/list/TestSheet.xlsx
+++ b/testdata/list/TestSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E1C270-7424-4392-825D-DD3465F8BF1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3A0D09-120E-443A-983D-64129611EEA4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,29 +21,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Nadpis</t>
   </si>
   <si>
-    <t>Row 1</t>
-  </si>
-  <si>
-    <t>Row 2</t>
-  </si>
-  <si>
-    <t>Row 3</t>
-  </si>
-  <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Entity2</t>
+  </si>
+  <si>
+    <t>Entity1</t>
+  </si>
+  <si>
+    <t>Entity3</t>
+  </si>
+  <si>
+    <t>Attr1</t>
+  </si>
+  <si>
+    <t>Attr2</t>
+  </si>
+  <si>
+    <t>Attr3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +72,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -96,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -104,6 +121,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,16 +402,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -405,7 +423,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -428,27 +446,45 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="C8" s="2">
+        <f>$B$8</f>
         <v>3</v>
       </c>
-      <c r="C5" s="2">
-        <f>$B$5</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="3">
-        <f>SUM(C3:C5)</f>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="3">
+        <f>SUM(C3:C8)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
         <f>'V100'!A1</f>
         <v>x</v>
       </c>
@@ -472,7 +508,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work in progress - everything in place but it still doesn't work...
</commit_message>
<xml_diff>
--- a/testdata/list/TestSheet.xlsx
+++ b/testdata/list/TestSheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3A0D09-120E-443A-983D-64129611EEA4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CD6947-F7E0-4F59-9A44-6F431ACF7B67}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Nadpis</t>
   </si>
@@ -118,10 +118,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,11 +415,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -434,57 +434,80 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>2</v>
       </c>
-      <c r="C4" s="2">
-        <f>$B$4</f>
+      <c r="C5" s="2">
+        <f>$B$5</f>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>3</v>
       </c>
-      <c r="C8" s="2">
-        <f>$B$8</f>
+      <c r="C9" s="2">
+        <f>$B$9</f>
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="3">
-        <f>SUM(C3:C8)</f>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="str">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="3">
+        <f>SUM(C3:C9)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
         <f>'V100'!A1</f>
         <v>x</v>
       </c>

</xml_diff>

<commit_message>
First version with working shift of references in formulas
</commit_message>
<xml_diff>
--- a/testdata/list/TestSheet.xlsx
+++ b/testdata/list/TestSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CD6947-F7E0-4F59-9A44-6F431ACF7B67}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07902B0F-2EAB-4BEB-8EFB-37FFE2F8AC04}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,17 +16,19 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Nadpis</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>Entity2</t>
@@ -402,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,7 +425,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -435,13 +437,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -453,25 +455,25 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -483,19 +485,19 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -504,12 +506,6 @@
       <c r="C13" s="3">
         <f>SUM(C3:C9)</f>
         <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="str">
-        <f>'V100'!A1</f>
-        <v>x</v>
       </c>
     </row>
   </sheetData>
@@ -528,13 +524,7 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>